<commit_message>
enhance the feature when open browser
</commit_message>
<xml_diff>
--- a/file/file_url.xlsx
+++ b/file/file_url.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\automate\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE9EE14-FC28-4317-91E4-8A7D6BC61BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F14D58-5637-4E51-8A42-CB1B8141572A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>https://www.youtube.com/watch?v=INGJh9DEaBM&amp;list=PL0Zuz27SZ-6MQri81d012LwP5jvFZ_scc&amp;index=7</t>
   </si>
   <si>
     <t>URL</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Python Lesson</t>
   </si>
 </sst>
 </file>
@@ -348,22 +360,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>